<commit_message>
feat: avances en limpieza de los datos, excluyendo quienes no hayan ingresado a crea
</commit_message>
<xml_diff>
--- a/Segregaciones/Estudiantes_solo_desconocidos.xlsx
+++ b/Segregaciones/Estudiantes_solo_desconocidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,26 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>cr_total_dias_ingreso</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>primera_conexion_crea</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>dias_de_conexion_dispositivo</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>primera_conexion_dispositivo</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>id_centro</t>
         </is>
       </c>

</xml_diff>

<commit_message>
feat(limpieza): datos de estudiantes
</commit_message>
<xml_diff>
--- a/Segregaciones/Estudiantes_solo_desconocidos.xlsx
+++ b/Segregaciones/Estudiantes_solo_desconocidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,6 +500,411 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1011825</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Estudiante</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1011825</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Estudiante</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1011825</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Estudiante</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1011825</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Estudiante</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>20</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1011825</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>9</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Estudiante</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>20</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1011825</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Estudiante</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>20</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1012812</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Estudiante</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>18</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1012812</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Estudiante</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>18</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1012812</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>DGES</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3er. CICLO EBI</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>desconocido</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Estudiante</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>18</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>